<commit_message>
Some minor changes in excel files and code
</commit_message>
<xml_diff>
--- a/Vishal Patel/WritetoEXCEL/Evaluation/BM25_scores_query_/BM25_scores_query_10_evaluation.xlsx
+++ b/Vishal Patel/WritetoEXCEL/Evaluation/BM25_scores_query_/BM25_scores_query_10_evaluation.xlsx
@@ -384,7 +384,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Precision on x recall on y</c:v>
+            <c:v>Precision vs recall</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -1016,6 +1016,7 @@
         </c:scaling>
         <c:delete val="false"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="true"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1026,6 +1027,8 @@
         <c:axId val="2"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="false"/>
         <c:axPos val="l"/>
@@ -1037,6 +1040,10 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:overlay val="false"/>
+    </c:legend>
     <c:plotVisOnly val="true"/>
   </c:chart>
   <c:printSettings>

</xml_diff>